<commit_message>
Refactored red green chart v2 code, added chart for end strength levels, changed some chart colors, added ability to rename HIFEs from SRCs from the HIFEs.xlsx workbook.
</commit_message>
<xml_diff>
--- a/HIFEs.xlsx
+++ b/HIFEs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">01225K000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77777K000</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -141,6 +147,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,12 +197,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,13 +227,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.28"/>
@@ -341,6 +357,14 @@
       </c>
       <c r="B15" s="0" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>